<commit_message>
Fix 'avenant caution' issue
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_4_2024.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_4_2024.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -429,10 +429,10 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>044/FES VILLE /AV6</v>
+        <v>665/FES 2</v>
       </c>
       <c r="B2" t="str">
-        <v>Direction régionale</v>
+        <v>Point de vente</v>
       </c>
       <c r="C2" t="str">
         <v>K5443645</v>
@@ -450,13 +450,13 @@
         <v>15</v>
       </c>
       <c r="H2">
-        <v>30000</v>
+        <v>10000</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>4500</v>
+        <v>1500</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -471,30 +471,30 @@
         <v>10000</v>
       </c>
       <c r="O2">
-        <v>25500</v>
+        <v>18500</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v xml:space="preserve"> </v>
+        <v>044/FES VILLE /AV6</v>
       </c>
       <c r="B3" t="str">
-        <v xml:space="preserve"> </v>
+        <v>Direction régionale</v>
       </c>
       <c r="C3" t="str">
-        <v xml:space="preserve"> </v>
+        <v>K5443645</v>
       </c>
       <c r="D3" t="str">
-        <v xml:space="preserve"> </v>
+        <v>KHADIJA LALA</v>
       </c>
       <c r="E3" t="str">
-        <v xml:space="preserve"> </v>
+        <v>non</v>
       </c>
       <c r="F3" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="G3" t="str">
-        <v xml:space="preserve"> </v>
+        <v>mensuelle</v>
+      </c>
+      <c r="G3">
+        <v>15</v>
       </c>
       <c r="H3">
         <v>30000</v>
@@ -519,11 +519,58 @@
       </c>
       <c r="O3">
         <v>25500</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="B4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="H4">
+        <v>40000</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>6000</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>20000</v>
+      </c>
+      <c r="O4">
+        <v>44000</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>